<commit_message>
changed a comment in main, changed matlab and excel files
</commit_message>
<xml_diff>
--- a/Lab 2/temperatureDataRising.xlsx
+++ b/Lab 2/temperatureDataRising.xlsx
@@ -155,7 +155,14 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.42554879792568301"/>
+          <c:y val="5.2159734738314888E-2"/>
+        </c:manualLayout>
+      </c:layout>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -208,7 +215,10 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="bg1">
+                  <a:lumMod val="50000"/>
+                  <a:alpha val="39000"/>
+                </a:schemeClr>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -4863,7 +4873,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent3"/>
+                <a:schemeClr val="accent4"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -7132,7 +7142,7 @@
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent4"/>
+                <a:schemeClr val="accent6"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -11362,31 +11372,127 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="340977448"/>
-        <c:axId val="426909208"/>
+        <c:axId val="291418640"/>
+        <c:axId val="291409232"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="340977448"/>
+        <c:axId val="291418640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
-        <c:delete val="1"/>
+        <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> of ticks</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
+        <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="426909208"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="291409232"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
+        <c:tickLblSkip val="50"/>
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="426909208"/>
+        <c:axId val="291409232"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="48"/>
           <c:min val="35"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -11405,6 +11511,73 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400"/>
+                  <a:t>Temperature</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" baseline="0"/>
+                  <a:t> (C</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
+                    <a:effectLst/>
+                  </a:rPr>
+                  <a:t>°)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US" sz="1400"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -11436,7 +11609,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="340977448"/>
+        <c:crossAx val="291418640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -11464,7 +11637,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -12077,16 +12250,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>4</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>20</xdr:col>
-      <xdr:colOff>581025</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>104775</xdr:rowOff>
+      <xdr:colOff>133350</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -12377,8 +12550,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E769"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="W4" sqref="W4"/>
+    <sheetView tabSelected="1" topLeftCell="D5" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="F29" sqref="F29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>